<commit_message>
[base] - [`startRecording()`]: prevent recording to commence if previous recording cannot be stopped.
[csv]
- [`compareExtended(var,profile,expected,actual)`]: minor improvement to reduce runtime exceptions. Also enforce `...compareExt.output.display` as required.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt_iter.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt_iter.xlsx
@@ -23,13 +23,13 @@
     <definedName name="csv">'#system'!$F$2:$F$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$G$2:$G$94</definedName>
+    <definedName name="desktop">'#system'!$G$2:$G$95</definedName>
     <definedName name="excel">'#system'!$H$2:$H$14</definedName>
     <definedName name="external">'#system'!$I$2:$I$5</definedName>
-    <definedName name="image">'#system'!$J$2:$J$6</definedName>
+    <definedName name="image">'#system'!$J$2:$J$7</definedName>
     <definedName name="io">'#system'!$K$2:$K$29</definedName>
     <definedName name="jms">'#system'!$L$2:$L$4</definedName>
-    <definedName name="json">'#system'!$M$2:$M$16</definedName>
+    <definedName name="json">'#system'!$M$2:$M$17</definedName>
     <definedName name="mail">'#system'!$P$2:$P$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
@@ -43,12 +43,12 @@
     <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
     <definedName name="step">'#system'!$X$2:$X$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$30</definedName>
-    <definedName name="web">'#system'!$Y$2:$Y$128</definedName>
+    <definedName name="web">'#system'!$Y$2:$Y$129</definedName>
     <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
     <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
-    <definedName name="xml">'#system'!$AD$2:$AD$21</definedName>
+    <definedName name="xml">'#system'!$AD$2:$AD$27</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
     <definedName name="macro">'#system'!$O$2:$O$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23567" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24114" uniqueCount="557">
   <si>
     <t>description</t>
   </si>
@@ -1706,13 +1706,46 @@
   <si>
     <t>assertTextNotContains(locator,text)</t>
   </si>
+  <si>
+    <t>saveModalDialogTextByLocator(var,locator)</t>
+  </si>
+  <si>
+    <t>typeKeys(os,keystrokes)</t>
+  </si>
+  <si>
+    <t>saveDiff(var,baseline,actual)</t>
+  </si>
+  <si>
+    <t>compact(var,json,removeEmpty)</t>
+  </si>
+  <si>
+    <t>clickAll(locator)</t>
+  </si>
+  <si>
+    <t>assertSoap(wsdl,xml)</t>
+  </si>
+  <si>
+    <t>assertSoapFaultCode(expected,xml)</t>
+  </si>
+  <si>
+    <t>assertSoapFaultString(expected,xml)</t>
+  </si>
+  <si>
+    <t>storeSoapFaultCode(var,xml)</t>
+  </si>
+  <si>
+    <t>storeSoapFaultDetail(var,xml)</t>
+  </si>
+  <si>
+    <t>storeSoapFaultString(var,xml)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="756" x14ac:knownFonts="1">
+  <fonts count="772" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6476,8 +6509,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1318">
+  <fills count="1345">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13942,8 +14076,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1347">
+  <borders count="1379">
     <border>
       <left/>
       <right/>
@@ -27339,6 +27626,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -27524,7 +28137,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="783">
+  <cellXfs count="799">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -29844,52 +30457,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1287" fontId="739" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="740" fillId="1290" borderId="1326" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1326" fillId="1290" fontId="740" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="741" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="741" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="742" fillId="1293" borderId="1330" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1330" fillId="1293" fontId="742" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="743" fillId="1296" borderId="1334" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1334" fillId="1296" fontId="743" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="744" fillId="1299" borderId="1334" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1334" fillId="1299" fontId="744" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="745" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="745" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="746" fillId="1302" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1302" fontId="746" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="747" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="747" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="748" fillId="1305" borderId="1338" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1338" fillId="1305" fontId="748" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="749" fillId="1308" borderId="1342" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1342" fillId="1308" fontId="749" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="750" fillId="1311" borderId="1346" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1346" fillId="1311" fontId="750" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="751" fillId="1311" borderId="1346" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1346" fillId="1311" fontId="751" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="752" fillId="1299" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1299" fontId="752" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="753" fillId="1314" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1314" fontId="753" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="754" fillId="1299" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1299" fontId="754" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="755" fillId="1317" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1317" fontId="755" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="756" fillId="1320" borderId="1354" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="757" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="758" fillId="1323" borderId="1358" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="759" fillId="1326" borderId="1362" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="760" fillId="1329" borderId="1366" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="761" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="762" fillId="1332" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="763" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="764" fillId="1335" borderId="1370" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="765" fillId="1326" borderId="1374" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="766" fillId="1338" borderId="1378" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="767" fillId="1338" borderId="1378" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="768" fillId="1329" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="769" fillId="1341" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="770" fillId="1329" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="771" fillId="1344" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -30244,7 +30905,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE128"/>
+  <dimension ref="A1:AE129"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -30766,6 +31427,9 @@
       <c r="H7" t="s">
         <v>461</v>
       </c>
+      <c r="J7" t="s">
+        <v>548</v>
+      </c>
       <c r="K7" t="s">
         <v>16</v>
       </c>
@@ -30806,7 +31470,7 @@
         <v>448</v>
       </c>
       <c r="AD7" t="s">
-        <v>233</v>
+        <v>551</v>
       </c>
     </row>
     <row r="8">
@@ -30862,7 +31526,7 @@
         <v>449</v>
       </c>
       <c r="AD8" t="s">
-        <v>234</v>
+        <v>552</v>
       </c>
     </row>
     <row r="9">
@@ -30909,7 +31573,7 @@
         <v>190</v>
       </c>
       <c r="AD9" t="s">
-        <v>235</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10">
@@ -30950,7 +31614,7 @@
         <v>191</v>
       </c>
       <c r="AD10" t="s">
-        <v>492</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11">
@@ -30988,7 +31652,7 @@
         <v>260</v>
       </c>
       <c r="AD11" t="s">
-        <v>509</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12">
@@ -31008,7 +31672,7 @@
         <v>398</v>
       </c>
       <c r="M12" t="s">
-        <v>454</v>
+        <v>549</v>
       </c>
       <c r="N12" t="s">
         <v>535</v>
@@ -31026,7 +31690,7 @@
         <v>192</v>
       </c>
       <c r="AD12" t="s">
-        <v>510</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13">
@@ -31046,7 +31710,7 @@
         <v>17</v>
       </c>
       <c r="M13" t="s">
-        <v>490</v>
+        <v>454</v>
       </c>
       <c r="Q13" t="s">
         <v>95</v>
@@ -31061,7 +31725,7 @@
         <v>193</v>
       </c>
       <c r="AD13" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
     </row>
     <row r="14">
@@ -31081,7 +31745,7 @@
         <v>42</v>
       </c>
       <c r="M14" t="s">
-        <v>39</v>
+        <v>490</v>
       </c>
       <c r="Q14" t="s">
         <v>96</v>
@@ -31096,7 +31760,7 @@
         <v>194</v>
       </c>
       <c r="AD14" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="15">
@@ -31113,7 +31777,7 @@
         <v>523</v>
       </c>
       <c r="M15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q15" t="s">
         <v>517</v>
@@ -31128,7 +31792,7 @@
         <v>195</v>
       </c>
       <c r="AD15" t="s">
-        <v>493</v>
+        <v>510</v>
       </c>
     </row>
     <row r="16">
@@ -31145,7 +31809,7 @@
         <v>82</v>
       </c>
       <c r="M16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="Q16" t="s">
         <v>518</v>
@@ -31160,7 +31824,7 @@
         <v>196</v>
       </c>
       <c r="AD16" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="17">
@@ -31176,6 +31840,9 @@
       <c r="K17" t="s">
         <v>83</v>
       </c>
+      <c r="M17" t="s">
+        <v>43</v>
+      </c>
       <c r="Y17" t="s">
         <v>519</v>
       </c>
@@ -31183,7 +31850,7 @@
         <v>479</v>
       </c>
       <c r="AD17" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="18">
@@ -31203,7 +31870,7 @@
         <v>106</v>
       </c>
       <c r="AD18" t="s">
-        <v>516</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19">
@@ -31223,7 +31890,7 @@
         <v>107</v>
       </c>
       <c r="AD19" t="s">
-        <v>236</v>
+        <v>511</v>
       </c>
     </row>
     <row r="20">
@@ -31243,7 +31910,7 @@
         <v>108</v>
       </c>
       <c r="AD20" t="s">
-        <v>237</v>
+        <v>512</v>
       </c>
     </row>
     <row r="21">
@@ -31263,7 +31930,7 @@
         <v>109</v>
       </c>
       <c r="AD21" t="s">
-        <v>238</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22">
@@ -31282,6 +31949,9 @@
       <c r="Y22" t="s">
         <v>500</v>
       </c>
+      <c r="AD22" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -31299,6 +31969,9 @@
       <c r="Y23" t="s">
         <v>111</v>
       </c>
+      <c r="AD23" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -31316,6 +31989,9 @@
       <c r="Y24" t="s">
         <v>112</v>
       </c>
+      <c r="AD24" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -31333,6 +32009,9 @@
       <c r="Y25" t="s">
         <v>113</v>
       </c>
+      <c r="AD25" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -31350,6 +32029,9 @@
       <c r="Y26" t="s">
         <v>114</v>
       </c>
+      <c r="AD26" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -31367,6 +32049,9 @@
       <c r="Y27" t="s">
         <v>115</v>
       </c>
+      <c r="AD27" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -31597,7 +32282,7 @@
         <v>369</v>
       </c>
       <c r="Y50" t="s">
-        <v>129</v>
+        <v>550</v>
       </c>
     </row>
     <row r="51">
@@ -31605,7 +32290,7 @@
         <v>303</v>
       </c>
       <c r="Y51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52">
@@ -31613,7 +32298,7 @@
         <v>357</v>
       </c>
       <c r="Y52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53">
@@ -31621,7 +32306,7 @@
         <v>332</v>
       </c>
       <c r="Y53" t="s">
-        <v>501</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54">
@@ -31629,7 +32314,7 @@
         <v>269</v>
       </c>
       <c r="Y54" t="s">
-        <v>481</v>
+        <v>501</v>
       </c>
     </row>
     <row r="55">
@@ -31637,7 +32322,7 @@
         <v>293</v>
       </c>
       <c r="Y55" t="s">
-        <v>132</v>
+        <v>481</v>
       </c>
     </row>
     <row r="56">
@@ -31645,7 +32330,7 @@
         <v>294</v>
       </c>
       <c r="Y56" t="s">
-        <v>347</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57">
@@ -31653,7 +32338,7 @@
         <v>295</v>
       </c>
       <c r="Y57" t="s">
-        <v>474</v>
+        <v>347</v>
       </c>
     </row>
     <row r="58">
@@ -31661,7 +32346,7 @@
         <v>304</v>
       </c>
       <c r="Y58" t="s">
-        <v>133</v>
+        <v>474</v>
       </c>
     </row>
     <row r="59">
@@ -31669,7 +32354,7 @@
         <v>313</v>
       </c>
       <c r="Y59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60">
@@ -31677,7 +32362,7 @@
         <v>338</v>
       </c>
       <c r="Y60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61">
@@ -31685,7 +32370,7 @@
         <v>310</v>
       </c>
       <c r="Y61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62">
@@ -31693,7 +32378,7 @@
         <v>311</v>
       </c>
       <c r="Y62" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63">
@@ -31701,7 +32386,7 @@
         <v>370</v>
       </c>
       <c r="Y63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64">
@@ -31709,7 +32394,7 @@
         <v>371</v>
       </c>
       <c r="Y64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65">
@@ -31717,7 +32402,7 @@
         <v>346</v>
       </c>
       <c r="Y65" t="s">
-        <v>451</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66">
@@ -31725,7 +32410,7 @@
         <v>314</v>
       </c>
       <c r="Y66" t="s">
-        <v>491</v>
+        <v>451</v>
       </c>
     </row>
     <row r="67">
@@ -31733,15 +32418,15 @@
         <v>270</v>
       </c>
       <c r="Y67" t="s">
-        <v>215</v>
+        <v>491</v>
       </c>
     </row>
     <row r="68">
       <c r="G68" t="s">
-        <v>354</v>
+        <v>546</v>
       </c>
       <c r="Y68" t="s">
-        <v>397</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69">
@@ -31749,7 +32434,7 @@
         <v>315</v>
       </c>
       <c r="Y69" t="s">
-        <v>456</v>
+        <v>397</v>
       </c>
     </row>
     <row r="70">
@@ -31757,7 +32442,7 @@
         <v>421</v>
       </c>
       <c r="Y70" t="s">
-        <v>140</v>
+        <v>456</v>
       </c>
     </row>
     <row r="71">
@@ -31765,7 +32450,7 @@
         <v>305</v>
       </c>
       <c r="Y71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72">
@@ -31773,7 +32458,7 @@
         <v>422</v>
       </c>
       <c r="Y72" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73">
@@ -31781,7 +32466,7 @@
         <v>263</v>
       </c>
       <c r="Y73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74">
@@ -31789,7 +32474,7 @@
         <v>526</v>
       </c>
       <c r="Y74" t="s">
-        <v>198</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75">
@@ -31797,7 +32482,7 @@
         <v>345</v>
       </c>
       <c r="Y75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="76">
@@ -31805,7 +32490,7 @@
         <v>281</v>
       </c>
       <c r="Y76" t="s">
-        <v>469</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77">
@@ -31813,7 +32498,7 @@
         <v>287</v>
       </c>
       <c r="Y77" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
     </row>
     <row r="78">
@@ -31821,7 +32506,7 @@
         <v>292</v>
       </c>
       <c r="Y78" t="s">
-        <v>144</v>
+        <v>485</v>
       </c>
     </row>
     <row r="79">
@@ -31829,7 +32514,7 @@
         <v>428</v>
       </c>
       <c r="Y79" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80">
@@ -31837,7 +32522,7 @@
         <v>333</v>
       </c>
       <c r="Y80" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81">
@@ -31845,7 +32530,7 @@
         <v>271</v>
       </c>
       <c r="Y81" t="s">
-        <v>513</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82">
@@ -31853,7 +32538,7 @@
         <v>282</v>
       </c>
       <c r="Y82" t="s">
-        <v>147</v>
+        <v>513</v>
       </c>
     </row>
     <row r="83">
@@ -31861,7 +32546,7 @@
         <v>288</v>
       </c>
       <c r="Y83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84">
@@ -31869,256 +32554,264 @@
         <v>277</v>
       </c>
       <c r="Y84" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85">
       <c r="G85" t="s">
-        <v>272</v>
+        <v>547</v>
       </c>
       <c r="Y85" t="s">
-        <v>502</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86">
       <c r="G86" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="Y86" t="s">
-        <v>201</v>
+        <v>502</v>
       </c>
     </row>
     <row r="87">
       <c r="G87" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="Y87" t="s">
-        <v>468</v>
+        <v>201</v>
       </c>
     </row>
     <row r="88">
       <c r="G88" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Y88" t="s">
-        <v>202</v>
+        <v>468</v>
       </c>
     </row>
     <row r="89">
       <c r="G89" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
       <c r="Y89" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="90">
       <c r="G90" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="Y90" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="91">
       <c r="G91" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="Y91" t="s">
-        <v>149</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92">
       <c r="G92" t="s">
-        <v>341</v>
+        <v>296</v>
       </c>
       <c r="Y92" t="s">
-        <v>204</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93">
       <c r="G93" t="s">
-        <v>278</v>
+        <v>341</v>
       </c>
       <c r="Y93" t="s">
-        <v>442</v>
+        <v>204</v>
       </c>
     </row>
     <row r="94">
       <c r="G94" t="s">
+        <v>278</v>
+      </c>
+      <c r="Y94" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="G95" t="s">
         <v>279</v>
       </c>
-      <c r="Y94" t="s">
+      <c r="Y95" t="s">
         <v>450</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="Y95" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="96">
       <c r="Y96" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="97">
       <c r="Y97" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="98">
       <c r="Y98" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99">
       <c r="Y99" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
     </row>
     <row r="100">
       <c r="Y100" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
     </row>
     <row r="101">
       <c r="Y101" t="s">
-        <v>524</v>
+        <v>209</v>
       </c>
     </row>
     <row r="102">
       <c r="Y102" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="103">
       <c r="Y103" t="s">
-        <v>150</v>
+        <v>527</v>
       </c>
     </row>
     <row r="104">
       <c r="Y104" t="s">
-        <v>528</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105">
       <c r="Y105" t="s">
-        <v>384</v>
+        <v>528</v>
       </c>
     </row>
     <row r="106">
       <c r="Y106" t="s">
-        <v>151</v>
+        <v>384</v>
       </c>
     </row>
     <row r="107">
       <c r="Y107" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108">
       <c r="Y108" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="109">
       <c r="Y109" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="110">
       <c r="Y110" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="111">
       <c r="Y111" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="112">
       <c r="Y112" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="113">
       <c r="Y113" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="114">
       <c r="Y114" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="115">
       <c r="Y115" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116">
       <c r="Y116" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117">
       <c r="Y117" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="118">
       <c r="Y118" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="119">
       <c r="Y119" t="s">
-        <v>457</v>
+        <v>163</v>
       </c>
     </row>
     <row r="120">
       <c r="Y120" t="s">
-        <v>164</v>
+        <v>457</v>
       </c>
     </row>
     <row r="121">
       <c r="Y121" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="122">
       <c r="Y122" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="123">
       <c r="Y123" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="124">
       <c r="Y124" t="s">
-        <v>47</v>
+        <v>167</v>
       </c>
     </row>
     <row r="125">
       <c r="Y125" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
     </row>
     <row r="126">
       <c r="Y126" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="127">
       <c r="Y127" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="128">
       <c r="Y128" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="Y129" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[system variables] - [`nexial.excel.recalcBeforeSave`]: **NEW** System variable to instruct Nexial to perform recalculation on Excel before saving it. - [`nexial.excel.retainCellType`]: **NEW** System variable to enable Nexial's attempt to retain the Excel cell type when writing data to it. More advanced cell type such as `OLE`, `CHART` is not yet support.
[expression]
- [EXCEL]: - **NEW** operation - `totalDataRow` - to expose the total number of row with data.

[excel commands]
- [`saveTotalDataCount(file,worksheet,saveVar)`]: **NEW** command to expose the total number of row with data.
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt_iter.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt_iter.xlsx
@@ -24,7 +24,7 @@
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
-    <definedName name="excel">'#system'!$I$2:$I$14</definedName>
+    <definedName name="excel">'#system'!$I$2:$I$15</definedName>
     <definedName name="external">'#system'!$J$2:$J$6</definedName>
     <definedName name="image">'#system'!$K$2:$K$7</definedName>
     <definedName name="io">'#system'!$L$2:$L$30</definedName>
@@ -35,7 +35,7 @@
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
     <definedName name="number">'#system'!$R$2:$R$16</definedName>
-    <definedName name="pdf">'#system'!$S$2:$S$16</definedName>
+    <definedName name="pdf">'#system'!$S$2:$S$17</definedName>
     <definedName name="rdbms">'#system'!$T$2:$T$7</definedName>
     <definedName name="redis">'#system'!$U$2:$U$10</definedName>
     <definedName name="sms">'#system'!$V$2:$V$2</definedName>
@@ -43,9 +43,9 @@
     <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$31</definedName>
-    <definedName name="web">'#system'!$Z$2:$Z$138</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$144</definedName>
     <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="webcookie">'#system'!$AB$2:$AB$10</definedName>
     <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
     <definedName name="ws.async">'#system'!$AD$2:$AD$8</definedName>
     <definedName name="xml">'#system'!$AE$2:$AE$27</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34727" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35303" uniqueCount="594">
   <si>
     <t>description</t>
   </si>
@@ -1822,13 +1822,43 @@
   <si>
     <t>saveBrowserVersion(var)</t>
   </si>
+  <si>
+    <t>saveTotalDataCount(file,worksheet,saveVar)</t>
+  </si>
+  <si>
+    <t>saveAsPdf(profile,content,file)</t>
+  </si>
+  <si>
+    <t>assertElementEnabled(locator)</t>
+  </si>
+  <si>
+    <t>saveTitle(var)</t>
+  </si>
+  <si>
+    <t>selectAllOptions(locator)</t>
+  </si>
+  <si>
+    <t>selectMultiByValue(locator,array)</t>
+  </si>
+  <si>
+    <t>switchBrowser(profile,config)</t>
+  </si>
+  <si>
+    <t>waitForElementsPresent(locators)</t>
+  </si>
+  <si>
+    <t>clearCookieFields(var,remove)</t>
+  </si>
+  <si>
+    <t>saveAllAsText(var,exclude)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1076" x14ac:knownFonts="1">
+  <fonts count="1092" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -8612,8 +8642,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1858">
+  <fills count="1885">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -19138,8 +19269,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1987">
+  <borders count="2019">
     <border>
       <left/>
       <right/>
@@ -32535,6 +32819,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -39240,7 +39850,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1103">
+  <cellXfs count="1119">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -42520,52 +43130,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1830" fontId="1059" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1060" fillId="1833" borderId="1962" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1061" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1962" fillId="1833" fontId="1060" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1061" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1062" fillId="1836" borderId="1966" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1966" fillId="1836" fontId="1062" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1063" fillId="1839" borderId="1970" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1970" fillId="1839" fontId="1063" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1064" fillId="1842" borderId="1974" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1974" fillId="1842" fontId="1064" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1065" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1065" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1066" fillId="1845" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1845" fontId="1066" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1067" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1068" fillId="1848" borderId="1978" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1069" fillId="1839" borderId="1982" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1070" fillId="1851" borderId="1986" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1071" fillId="1851" borderId="1986" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1072" fillId="1842" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1073" fillId="1854" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1074" fillId="1842" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1075" fillId="1857" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1067" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1978" fillId="1848" fontId="1068" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1982" fillId="1839" fontId="1069" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1986" fillId="1851" fontId="1070" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1986" fillId="1851" fontId="1071" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1842" fontId="1072" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1854" fontId="1073" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1842" fontId="1074" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1857" fontId="1075" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1076" fillId="1860" borderId="1994" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1077" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1078" fillId="1863" borderId="1998" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1079" fillId="1866" borderId="2002" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1080" fillId="1869" borderId="2006" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1081" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1082" fillId="1872" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1083" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1084" fillId="1875" borderId="2010" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1085" fillId="1866" borderId="2014" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1086" fillId="1878" borderId="2018" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1087" fillId="1878" borderId="2018" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1088" fillId="1869" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1089" fillId="1881" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1090" fillId="1869" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1091" fillId="1884" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -42920,7 +43578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF138"/>
+  <dimension ref="A1:AF144"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -43352,7 +44010,7 @@
         <v>175</v>
       </c>
       <c r="AB5" t="s">
-        <v>180</v>
+        <v>592</v>
       </c>
       <c r="AC5" t="s">
         <v>186</v>
@@ -43423,7 +44081,7 @@
         <v>458</v>
       </c>
       <c r="AB6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AC6" t="s">
         <v>187</v>
@@ -43485,7 +44143,7 @@
         <v>459</v>
       </c>
       <c r="AB7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AC7" t="s">
         <v>188</v>
@@ -43541,7 +44199,7 @@
         <v>176</v>
       </c>
       <c r="AB8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AC8" t="s">
         <v>189</v>
@@ -43593,6 +44251,9 @@
       <c r="Z9" t="s">
         <v>210</v>
       </c>
+      <c r="AB9" t="s">
+        <v>183</v>
+      </c>
       <c r="AC9" t="s">
         <v>190</v>
       </c>
@@ -43611,7 +44272,7 @@
         <v>307</v>
       </c>
       <c r="I10" t="s">
-        <v>466</v>
+        <v>584</v>
       </c>
       <c r="L10" t="s">
         <v>81</v>
@@ -43634,6 +44295,9 @@
       <c r="Z10" t="s">
         <v>258</v>
       </c>
+      <c r="AB10" t="s">
+        <v>593</v>
+      </c>
       <c r="AC10" t="s">
         <v>191</v>
       </c>
@@ -43652,7 +44316,7 @@
         <v>353</v>
       </c>
       <c r="I11" t="s">
-        <v>323</v>
+        <v>466</v>
       </c>
       <c r="L11" t="s">
         <v>38</v>
@@ -43690,7 +44354,7 @@
         <v>275</v>
       </c>
       <c r="I12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L12" t="s">
         <v>522</v>
@@ -43728,7 +44392,7 @@
         <v>264</v>
       </c>
       <c r="I13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L13" t="s">
         <v>398</v>
@@ -43740,7 +44404,7 @@
         <v>95</v>
       </c>
       <c r="S13" t="s">
-        <v>255</v>
+        <v>585</v>
       </c>
       <c r="Z13" t="s">
         <v>327</v>
@@ -43763,7 +44427,7 @@
         <v>317</v>
       </c>
       <c r="I14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L14" t="s">
         <v>17</v>
@@ -43775,7 +44439,7 @@
         <v>96</v>
       </c>
       <c r="S14" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="Z14" t="s">
         <v>104</v>
@@ -43796,6 +44460,9 @@
       </c>
       <c r="H15" t="s">
         <v>265</v>
+      </c>
+      <c r="I15" t="s">
+        <v>326</v>
       </c>
       <c r="L15" t="s">
         <v>42</v>
@@ -43807,10 +44474,10 @@
         <v>517</v>
       </c>
       <c r="S15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Z15" t="s">
-        <v>105</v>
+        <v>586</v>
       </c>
       <c r="AC15" t="s">
         <v>195</v>
@@ -43839,10 +44506,10 @@
         <v>518</v>
       </c>
       <c r="S16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Z16" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="AC16" t="s">
         <v>196</v>
@@ -43867,8 +44534,11 @@
       <c r="N17" t="s">
         <v>40</v>
       </c>
+      <c r="S17" t="s">
+        <v>253</v>
+      </c>
       <c r="Z17" t="s">
-        <v>519</v>
+        <v>76</v>
       </c>
       <c r="AC17" t="s">
         <v>479</v>
@@ -43894,7 +44564,7 @@
         <v>43</v>
       </c>
       <c r="Z18" t="s">
-        <v>106</v>
+        <v>519</v>
       </c>
       <c r="AE18" t="s">
         <v>493</v>
@@ -43914,7 +44584,7 @@
         <v>471</v>
       </c>
       <c r="Z19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AE19" t="s">
         <v>511</v>
@@ -43934,7 +44604,7 @@
         <v>84</v>
       </c>
       <c r="Z20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AE20" t="s">
         <v>512</v>
@@ -43954,7 +44624,7 @@
         <v>85</v>
       </c>
       <c r="Z21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AE21" t="s">
         <v>516</v>
@@ -43974,7 +44644,7 @@
         <v>577</v>
       </c>
       <c r="Z22" t="s">
-        <v>500</v>
+        <v>109</v>
       </c>
       <c r="AE22" t="s">
         <v>236</v>
@@ -43994,7 +44664,7 @@
         <v>488</v>
       </c>
       <c r="Z23" t="s">
-        <v>111</v>
+        <v>500</v>
       </c>
       <c r="AE23" t="s">
         <v>554</v>
@@ -44014,7 +44684,7 @@
         <v>44</v>
       </c>
       <c r="Z24" t="s">
-        <v>563</v>
+        <v>111</v>
       </c>
       <c r="AE24" t="s">
         <v>555</v>
@@ -44034,7 +44704,7 @@
         <v>400</v>
       </c>
       <c r="Z25" t="s">
-        <v>112</v>
+        <v>563</v>
       </c>
       <c r="AE25" t="s">
         <v>556</v>
@@ -44054,7 +44724,7 @@
         <v>541</v>
       </c>
       <c r="Z26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AE26" t="s">
         <v>237</v>
@@ -44074,7 +44744,7 @@
         <v>86</v>
       </c>
       <c r="Z27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AE27" t="s">
         <v>238</v>
@@ -44094,7 +44764,7 @@
         <v>453</v>
       </c>
       <c r="Z28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29">
@@ -44111,7 +44781,7 @@
         <v>45</v>
       </c>
       <c r="Z29" t="s">
-        <v>328</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30">
@@ -44128,7 +44798,7 @@
         <v>46</v>
       </c>
       <c r="Z30" t="s">
-        <v>116</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31">
@@ -44142,7 +44812,7 @@
         <v>217</v>
       </c>
       <c r="Z31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32">
@@ -44153,7 +44823,7 @@
         <v>276</v>
       </c>
       <c r="Z32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33">
@@ -44164,7 +44834,7 @@
         <v>286</v>
       </c>
       <c r="Z33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34">
@@ -44175,7 +44845,7 @@
         <v>525</v>
       </c>
       <c r="Z34" t="s">
-        <v>564</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35">
@@ -44186,7 +44856,7 @@
         <v>261</v>
       </c>
       <c r="Z35" t="s">
-        <v>120</v>
+        <v>564</v>
       </c>
     </row>
     <row r="36">
@@ -44197,7 +44867,7 @@
         <v>331</v>
       </c>
       <c r="Z36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37">
@@ -44208,7 +44878,7 @@
         <v>308</v>
       </c>
       <c r="Z37" t="s">
-        <v>211</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38">
@@ -44219,7 +44889,7 @@
         <v>262</v>
       </c>
       <c r="Z38" t="s">
-        <v>122</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39">
@@ -44230,7 +44900,7 @@
         <v>309</v>
       </c>
       <c r="Z39" t="s">
-        <v>339</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40">
@@ -44238,7 +44908,7 @@
         <v>268</v>
       </c>
       <c r="Z40" t="s">
-        <v>440</v>
+        <v>339</v>
       </c>
     </row>
     <row r="41">
@@ -44246,7 +44916,7 @@
         <v>79</v>
       </c>
       <c r="Z41" t="s">
-        <v>574</v>
+        <v>440</v>
       </c>
     </row>
     <row r="42">
@@ -44254,7 +44924,7 @@
         <v>213</v>
       </c>
       <c r="Z42" t="s">
-        <v>401</v>
+        <v>574</v>
       </c>
     </row>
     <row r="43">
@@ -44262,7 +44932,7 @@
         <v>560</v>
       </c>
       <c r="Z43" t="s">
-        <v>123</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44">
@@ -44270,7 +44940,7 @@
         <v>290</v>
       </c>
       <c r="Z44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45">
@@ -44278,7 +44948,7 @@
         <v>301</v>
       </c>
       <c r="Z45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46">
@@ -44286,7 +44956,7 @@
         <v>302</v>
       </c>
       <c r="Z46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47">
@@ -44294,7 +44964,7 @@
         <v>344</v>
       </c>
       <c r="Z47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48">
@@ -44302,7 +44972,7 @@
         <v>343</v>
       </c>
       <c r="Z48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49">
@@ -44310,7 +44980,7 @@
         <v>212</v>
       </c>
       <c r="Z49" t="s">
-        <v>455</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50">
@@ -44318,7 +44988,7 @@
         <v>321</v>
       </c>
       <c r="Z50" t="s">
-        <v>214</v>
+        <v>455</v>
       </c>
     </row>
     <row r="51">
@@ -44326,7 +44996,7 @@
         <v>340</v>
       </c>
       <c r="Z51" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52">
@@ -44334,7 +45004,7 @@
         <v>369</v>
       </c>
       <c r="Z52" t="s">
-        <v>550</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53">
@@ -44342,7 +45012,7 @@
         <v>303</v>
       </c>
       <c r="Z53" t="s">
-        <v>129</v>
+        <v>550</v>
       </c>
     </row>
     <row r="54">
@@ -44350,7 +45020,7 @@
         <v>357</v>
       </c>
       <c r="Z54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55">
@@ -44358,7 +45028,7 @@
         <v>332</v>
       </c>
       <c r="Z55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56">
@@ -44366,7 +45036,7 @@
         <v>269</v>
       </c>
       <c r="Z56" t="s">
-        <v>501</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57">
@@ -44374,7 +45044,7 @@
         <v>293</v>
       </c>
       <c r="Z57" t="s">
-        <v>481</v>
+        <v>501</v>
       </c>
     </row>
     <row r="58">
@@ -44382,7 +45052,7 @@
         <v>294</v>
       </c>
       <c r="Z58" t="s">
-        <v>132</v>
+        <v>481</v>
       </c>
     </row>
     <row r="59">
@@ -44390,7 +45060,7 @@
         <v>561</v>
       </c>
       <c r="Z59" t="s">
-        <v>347</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60">
@@ -44398,7 +45068,7 @@
         <v>295</v>
       </c>
       <c r="Z60" t="s">
-        <v>474</v>
+        <v>347</v>
       </c>
     </row>
     <row r="61">
@@ -44406,7 +45076,7 @@
         <v>304</v>
       </c>
       <c r="Z61" t="s">
-        <v>133</v>
+        <v>474</v>
       </c>
     </row>
     <row r="62">
@@ -44414,7 +45084,7 @@
         <v>313</v>
       </c>
       <c r="Z62" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63">
@@ -44422,7 +45092,7 @@
         <v>338</v>
       </c>
       <c r="Z63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64">
@@ -44430,7 +45100,7 @@
         <v>310</v>
       </c>
       <c r="Z64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65">
@@ -44438,7 +45108,7 @@
         <v>311</v>
       </c>
       <c r="Z65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66">
@@ -44446,7 +45116,7 @@
         <v>370</v>
       </c>
       <c r="Z66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67">
@@ -44454,7 +45124,7 @@
         <v>371</v>
       </c>
       <c r="Z67" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68">
@@ -44462,7 +45132,7 @@
         <v>346</v>
       </c>
       <c r="Z68" t="s">
-        <v>451</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69">
@@ -44470,7 +45140,7 @@
         <v>314</v>
       </c>
       <c r="Z69" t="s">
-        <v>491</v>
+        <v>451</v>
       </c>
     </row>
     <row r="70">
@@ -44478,7 +45148,7 @@
         <v>270</v>
       </c>
       <c r="Z70" t="s">
-        <v>215</v>
+        <v>491</v>
       </c>
     </row>
     <row r="71">
@@ -44486,7 +45156,7 @@
         <v>546</v>
       </c>
       <c r="Z71" t="s">
-        <v>397</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72">
@@ -44494,7 +45164,7 @@
         <v>315</v>
       </c>
       <c r="Z72" t="s">
-        <v>456</v>
+        <v>397</v>
       </c>
     </row>
     <row r="73">
@@ -44502,7 +45172,7 @@
         <v>421</v>
       </c>
       <c r="Z73" t="s">
-        <v>140</v>
+        <v>456</v>
       </c>
     </row>
     <row r="74">
@@ -44510,7 +45180,7 @@
         <v>305</v>
       </c>
       <c r="Z74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75">
@@ -44518,7 +45188,7 @@
         <v>422</v>
       </c>
       <c r="Z75" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76">
@@ -44526,7 +45196,7 @@
         <v>263</v>
       </c>
       <c r="Z76" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77">
@@ -44534,7 +45204,7 @@
         <v>526</v>
       </c>
       <c r="Z77" t="s">
-        <v>198</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78">
@@ -44542,7 +45212,7 @@
         <v>345</v>
       </c>
       <c r="Z78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79">
@@ -44550,7 +45220,7 @@
         <v>281</v>
       </c>
       <c r="Z79" t="s">
-        <v>469</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80">
@@ -44558,7 +45228,7 @@
         <v>287</v>
       </c>
       <c r="Z80" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
     </row>
     <row r="81">
@@ -44566,7 +45236,7 @@
         <v>292</v>
       </c>
       <c r="Z81" t="s">
-        <v>144</v>
+        <v>485</v>
       </c>
     </row>
     <row r="82">
@@ -44574,7 +45244,7 @@
         <v>428</v>
       </c>
       <c r="Z82" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83">
@@ -44582,7 +45252,7 @@
         <v>333</v>
       </c>
       <c r="Z83" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84">
@@ -44590,7 +45260,7 @@
         <v>271</v>
       </c>
       <c r="Z84" t="s">
-        <v>513</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85">
@@ -44598,7 +45268,7 @@
         <v>282</v>
       </c>
       <c r="Z85" t="s">
-        <v>147</v>
+        <v>513</v>
       </c>
     </row>
     <row r="86">
@@ -44606,7 +45276,7 @@
         <v>288</v>
       </c>
       <c r="Z86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87">
@@ -44614,7 +45284,7 @@
         <v>277</v>
       </c>
       <c r="Z87" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88">
@@ -44622,7 +45292,7 @@
         <v>547</v>
       </c>
       <c r="Z88" t="s">
-        <v>502</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89">
@@ -44630,7 +45300,7 @@
         <v>272</v>
       </c>
       <c r="Z89" t="s">
-        <v>583</v>
+        <v>502</v>
       </c>
     </row>
     <row r="90">
@@ -44638,7 +45308,7 @@
         <v>289</v>
       </c>
       <c r="Z90" t="s">
-        <v>201</v>
+        <v>583</v>
       </c>
     </row>
     <row r="91">
@@ -44646,7 +45316,7 @@
         <v>273</v>
       </c>
       <c r="Z91" t="s">
-        <v>468</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92">
@@ -44654,7 +45324,7 @@
         <v>274</v>
       </c>
       <c r="Z92" t="s">
-        <v>202</v>
+        <v>468</v>
       </c>
     </row>
     <row r="93">
@@ -44662,7 +45332,7 @@
         <v>306</v>
       </c>
       <c r="Z93" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="94">
@@ -44670,7 +45340,7 @@
         <v>312</v>
       </c>
       <c r="Z94" t="s">
-        <v>568</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95">
@@ -44678,7 +45348,7 @@
         <v>296</v>
       </c>
       <c r="Z95" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="96">
@@ -44686,7 +45356,7 @@
         <v>341</v>
       </c>
       <c r="Z96" t="s">
-        <v>216</v>
+        <v>569</v>
       </c>
     </row>
     <row r="97">
@@ -44694,7 +45364,7 @@
         <v>278</v>
       </c>
       <c r="Z97" t="s">
-        <v>149</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98">
@@ -44702,206 +45372,236 @@
         <v>279</v>
       </c>
       <c r="Z98" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="Z99" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="99">
-      <c r="Z99" t="s">
+    <row r="100">
+      <c r="Z100" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="100">
-      <c r="Z100" t="s">
+    <row r="101">
+      <c r="Z101" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="101">
-      <c r="Z101" t="s">
+    <row r="102">
+      <c r="Z102" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="102">
-      <c r="Z102" t="s">
+    <row r="103">
+      <c r="Z103" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="103">
-      <c r="Z103" t="s">
+    <row r="104">
+      <c r="Z104" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="104">
-      <c r="Z104" t="s">
+    <row r="105">
+      <c r="Z105" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="105">
-      <c r="Z105" t="s">
+    <row r="106">
+      <c r="Z106" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="106">
-      <c r="Z106" t="s">
+    <row r="107">
+      <c r="Z107" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="107">
-      <c r="Z107" t="s">
+    <row r="108">
+      <c r="Z108" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="108">
-      <c r="Z108" t="s">
+    <row r="109">
+      <c r="Z109" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="Z110" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="109">
-      <c r="Z109" t="s">
+    <row r="111">
+      <c r="Z111" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="110">
-      <c r="Z110" t="s">
+    <row r="112">
+      <c r="Z112" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="111">
-      <c r="Z111" t="s">
+    <row r="113">
+      <c r="Z113" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="112">
-      <c r="Z112" t="s">
+    <row r="114">
+      <c r="Z114" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="113">
-      <c r="Z113" t="s">
+    <row r="115">
+      <c r="Z115" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="114">
-      <c r="Z114" t="s">
+    <row r="116">
+      <c r="Z116" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="115">
-      <c r="Z115" t="s">
+    <row r="117">
+      <c r="Z117" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="116">
-      <c r="Z116" t="s">
+    <row r="118">
+      <c r="Z118" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="117">
-      <c r="Z117" t="s">
+    <row r="119">
+      <c r="Z119" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="Z120" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="118">
-      <c r="Z118" t="s">
+    <row r="121">
+      <c r="Z121" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="119">
-      <c r="Z119" t="s">
+    <row r="122">
+      <c r="Z122" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="Z123" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="120">
-      <c r="Z120" t="s">
+    <row r="124">
+      <c r="Z124" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="121">
-      <c r="Z121" t="s">
+    <row r="125">
+      <c r="Z125" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="122">
-      <c r="Z122" t="s">
+    <row r="126">
+      <c r="Z126" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="123">
-      <c r="Z123" t="s">
+    <row r="127">
+      <c r="Z127" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="124">
-      <c r="Z124" t="s">
+    <row r="128">
+      <c r="Z128" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="125">
-      <c r="Z125" t="s">
+    <row r="129">
+      <c r="Z129" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="Z130" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="126">
-      <c r="Z126" t="s">
+    <row r="131">
+      <c r="Z131" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="127">
-      <c r="Z127" t="s">
+    <row r="132">
+      <c r="Z132" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="128">
-      <c r="Z128" t="s">
+    <row r="133">
+      <c r="Z133" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="129">
-      <c r="Z129" t="s">
+    <row r="134">
+      <c r="Z134" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="130">
-      <c r="Z130" t="s">
+    <row r="135">
+      <c r="Z135" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="131">
-      <c r="Z131" t="s">
+    <row r="136">
+      <c r="Z136" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="132">
-      <c r="Z132" t="s">
+    <row r="137">
+      <c r="Z137" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="133">
-      <c r="Z133" t="s">
+    <row r="138">
+      <c r="Z138" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="134">
-      <c r="Z134" t="s">
+    <row r="139">
+      <c r="Z139" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="135">
-      <c r="Z135" t="s">
+    <row r="140">
+      <c r="Z140" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="136">
-      <c r="Z136" t="s">
+    <row r="141">
+      <c r="Z141" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="Z142" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="137">
-      <c r="Z137" t="s">
+    <row r="143">
+      <c r="Z143" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="138">
-      <c r="Z138" t="s">
+    <row r="144">
+      <c r="Z144" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed failed unit tests due to outdated scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt_iter.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt_iter.xlsx
@@ -24,7 +24,7 @@
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
-    <definedName name="excel">'#system'!$I$2:$I$15</definedName>
+    <definedName name="excel">'#system'!$I$2:$I$16</definedName>
     <definedName name="external">'#system'!$J$2:$J$6</definedName>
     <definedName name="image">'#system'!$K$2:$K$7</definedName>
     <definedName name="io">'#system'!$L$2:$L$30</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35303" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35880" uniqueCount="596">
   <si>
     <t>description</t>
   </si>
@@ -1852,13 +1852,19 @@
   <si>
     <t>saveAllAsText(var,exclude)</t>
   </si>
+  <si>
+    <t>saveTotalColumnCount(file,worksheet,row,saveVar)</t>
+  </si>
+  <si>
+    <t>saveTotalRowCount(file,worksheet,saveVar)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1092" x14ac:knownFonts="1">
+  <fonts count="1108" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -8743,8 +8749,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1885">
+  <fills count="1912">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -19422,8 +19529,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2019">
+  <borders count="2051">
     <border>
       <left/>
       <right/>
@@ -32819,6 +33079,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -39850,7 +40436,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1119">
+  <cellXfs count="1135">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -43178,52 +43764,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1857" fontId="1075" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1076" fillId="1860" borderId="1994" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1077" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1994" fillId="1860" fontId="1076" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1077" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1078" fillId="1863" borderId="1998" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1998" fillId="1863" fontId="1078" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1079" fillId="1866" borderId="2002" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2002" fillId="1866" fontId="1079" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1080" fillId="1869" borderId="2006" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2006" fillId="1869" fontId="1080" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1081" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1081" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1082" fillId="1872" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1872" fontId="1082" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1083" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1084" fillId="1875" borderId="2010" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1085" fillId="1866" borderId="2014" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1086" fillId="1878" borderId="2018" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1087" fillId="1878" borderId="2018" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1088" fillId="1869" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1089" fillId="1881" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1090" fillId="1869" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1091" fillId="1884" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1083" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2010" fillId="1875" fontId="1084" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2014" fillId="1866" fontId="1085" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2018" fillId="1878" fontId="1086" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2018" fillId="1878" fontId="1087" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1869" fontId="1088" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1881" fontId="1089" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1869" fontId="1090" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1884" fontId="1091" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1092" fillId="1887" borderId="2026" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1093" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1094" fillId="1890" borderId="2030" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1095" fillId="1893" borderId="2034" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1096" fillId="1896" borderId="2038" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1097" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1098" fillId="1899" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1099" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1100" fillId="1902" borderId="2042" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1101" fillId="1893" borderId="2046" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1102" fillId="1905" borderId="2050" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1103" fillId="1905" borderId="2050" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1104" fillId="1896" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1105" fillId="1908" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1106" fillId="1896" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1107" fillId="1911" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -44272,7 +44906,7 @@
         <v>307</v>
       </c>
       <c r="I10" t="s">
-        <v>584</v>
+        <v>594</v>
       </c>
       <c r="L10" t="s">
         <v>81</v>
@@ -44316,7 +44950,7 @@
         <v>353</v>
       </c>
       <c r="I11" t="s">
-        <v>466</v>
+        <v>595</v>
       </c>
       <c r="L11" t="s">
         <v>38</v>
@@ -44354,7 +44988,7 @@
         <v>275</v>
       </c>
       <c r="I12" t="s">
-        <v>323</v>
+        <v>466</v>
       </c>
       <c r="L12" t="s">
         <v>522</v>
@@ -44392,7 +45026,7 @@
         <v>264</v>
       </c>
       <c r="I13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L13" t="s">
         <v>398</v>
@@ -44427,7 +45061,7 @@
         <v>317</v>
       </c>
       <c r="I14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L14" t="s">
         <v>17</v>
@@ -44462,7 +45096,7 @@
         <v>265</v>
       </c>
       <c r="I15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L15" t="s">
         <v>42</v>
@@ -44495,6 +45129,9 @@
       </c>
       <c r="H16" t="s">
         <v>266</v>
+      </c>
+      <c r="I16" t="s">
+        <v>326</v>
       </c>
       <c r="L16" t="s">
         <v>523</v>

</xml_diff>

<commit_message>
[rdbms commands] - improve console logs to aid in troubleshooting - [`assertResultMatch(var,columns,search)`] - *NEW* command to verify that a query result contains certain data. `search` parameter can be prefixed with `REGEX:` for regular expression check, `CONTAIN:` for substring check, or "as is" for equality check. - [`assertResultNotMatch(var,columns,search)`] - *NEW* command to verify that a query result DOES NOT contains certain data. `search` parameter can be prefixed with `REGEX:` for regular expression check, `CONTAIN:` for substring check, or "as is" for equality check.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt_iter.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_ExecInterrupt_iter.xlsx
@@ -36,14 +36,14 @@
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
     <definedName name="number">'#system'!$R$2:$R$16</definedName>
     <definedName name="pdf">'#system'!$S$2:$S$17</definedName>
-    <definedName name="rdbms">'#system'!$T$2:$T$7</definedName>
+    <definedName name="rdbms">'#system'!$T$2:$T$9</definedName>
     <definedName name="redis">'#system'!$U$2:$U$10</definedName>
     <definedName name="sms">'#system'!$V$2:$V$2</definedName>
     <definedName name="sound">'#system'!$W$2:$W$5</definedName>
     <definedName name="ssh">'#system'!$X$2:$X$9</definedName>
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$32</definedName>
-    <definedName name="web">'#system'!$AA$2:$AA$144</definedName>
+    <definedName name="web">'#system'!$AA$2:$AA$145</definedName>
     <definedName name="webalert">'#system'!$AB$2:$AB$8</definedName>
     <definedName name="webcookie">'#system'!$AC$2:$AC$10</definedName>
     <definedName name="ws">'#system'!$AD$2:$AD$17</definedName>
@@ -52,10 +52,11 @@
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
     <definedName name="macro">'#system'!$P$2:$P$4</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
-    <definedName name="localdb">'#system'!$O$2:$O$12</definedName>
+    <definedName name="localdb">'#system'!$O$2:$O$13</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
     <definedName name="aws.vision">'#system'!$E$2:$E$2</definedName>
     <definedName name="tn.5250">'#system'!$Z$2:$Z$6</definedName>
+    <definedName name="step.inTime">'#system'!$Z$2:$Z$4</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37050" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37637" uniqueCount="614">
   <si>
     <t>description</t>
   </si>
@@ -1883,13 +1884,43 @@
   <si>
     <t>ocr(image,saveVar)</t>
   </si>
+  <si>
+    <t>step.inTime</t>
+  </si>
+  <si>
+    <t>queryAsCSV(var,sql)</t>
+  </si>
+  <si>
+    <t>assertResultMatch(var,columns,search)</t>
+  </si>
+  <si>
+    <t>assertResultNotMatch(var,columns,search)</t>
+  </si>
+  <si>
+    <t>observe(prompt,waitMs)</t>
+  </si>
+  <si>
+    <t>perform(instructions,waitMs)</t>
+  </si>
+  <si>
+    <t>validate(prompt,responses,passResponses,waitMs)</t>
+  </si>
+  <si>
+    <t>assertElementDisabled(locator)</t>
+  </si>
+  <si>
+    <t>checkAll(locator,waitMs)</t>
+  </si>
+  <si>
+    <t>uncheckAll(locator,waitMs)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1140" x14ac:knownFonts="1">
+  <fonts count="1156" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -9077,8 +9108,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1966">
+  <fills count="1993">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -20215,8 +20347,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2115">
+  <borders count="2147">
     <border>
       <left/>
       <right/>
@@ -33612,6 +33897,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -41621,7 +42232,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1167">
+  <cellXfs count="1183">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -45093,52 +45704,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1938" fontId="1123" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1124" fillId="1941" borderId="2090" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1125" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2090" fillId="1941" fontId="1124" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1125" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1126" fillId="1944" borderId="2094" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2094" fillId="1944" fontId="1126" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1127" fillId="1947" borderId="2098" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2098" fillId="1947" fontId="1127" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1128" fillId="1950" borderId="2102" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2102" fillId="1950" fontId="1128" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1129" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1129" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1130" fillId="1953" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1953" fontId="1130" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1131" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1132" fillId="1956" borderId="2106" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1133" fillId="1947" borderId="2110" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1134" fillId="1959" borderId="2114" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1135" fillId="1959" borderId="2114" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1136" fillId="1950" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1137" fillId="1962" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1138" fillId="1950" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1139" fillId="1965" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1131" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2106" fillId="1956" fontId="1132" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2110" fillId="1947" fontId="1133" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2114" fillId="1959" fontId="1134" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2114" fillId="1959" fontId="1135" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1950" fontId="1136" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1962" fontId="1137" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1950" fontId="1138" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1965" fontId="1139" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1140" fillId="1968" borderId="2122" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1141" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1142" fillId="1971" borderId="2126" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1143" fillId="1974" borderId="2130" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1144" fillId="1977" borderId="2134" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1145" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1146" fillId="1980" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1147" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1148" fillId="1983" borderId="2138" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1149" fillId="1974" borderId="2142" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1150" fillId="1986" borderId="2146" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1151" fillId="1986" borderId="2146" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1152" fillId="1977" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1153" fillId="1989" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1154" fillId="1977" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1155" fillId="1992" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -45493,7 +46152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG144"/>
+  <dimension ref="A1:AG145"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -45581,7 +46240,7 @@
         <v>407</v>
       </c>
       <c r="Z1" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="AA1" t="s">
         <v>55</v>
@@ -45661,7 +46320,7 @@
         <v>254</v>
       </c>
       <c r="T2" t="s">
-        <v>218</v>
+        <v>606</v>
       </c>
       <c r="U2" t="s">
         <v>412</v>
@@ -45679,7 +46338,7 @@
         <v>408</v>
       </c>
       <c r="Z2" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
       <c r="AA2" t="s">
         <v>98</v>
@@ -45753,7 +46412,7 @@
         <v>241</v>
       </c>
       <c r="T3" t="s">
-        <v>219</v>
+        <v>607</v>
       </c>
       <c r="U3" t="s">
         <v>413</v>
@@ -45768,7 +46427,7 @@
         <v>409</v>
       </c>
       <c r="Z3" t="s">
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="AA3" t="s">
         <v>99</v>
@@ -45839,7 +46498,7 @@
         <v>242</v>
       </c>
       <c r="T4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U4" t="s">
         <v>414</v>
@@ -45854,7 +46513,7 @@
         <v>410</v>
       </c>
       <c r="Z4" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="AA4" t="s">
         <v>580</v>
@@ -45919,7 +46578,7 @@
         <v>243</v>
       </c>
       <c r="T5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="U5" t="s">
         <v>415</v>
@@ -45929,9 +46588,6 @@
       </c>
       <c r="X5" t="s">
         <v>360</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>601</v>
       </c>
       <c r="AA5" t="s">
         <v>573</v>
@@ -45996,16 +46652,13 @@
         <v>244</v>
       </c>
       <c r="T6" t="s">
-        <v>399</v>
+        <v>220</v>
       </c>
       <c r="U6" t="s">
         <v>416</v>
       </c>
       <c r="X6" t="s">
         <v>362</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>602</v>
       </c>
       <c r="AA6" t="s">
         <v>100</v>
@@ -46061,7 +46714,7 @@
         <v>245</v>
       </c>
       <c r="T7" t="s">
-        <v>434</v>
+        <v>221</v>
       </c>
       <c r="U7" t="s">
         <v>417</v>
@@ -46122,6 +46775,9 @@
       <c r="S8" t="s">
         <v>246</v>
       </c>
+      <c r="T8" t="s">
+        <v>399</v>
+      </c>
       <c r="U8" t="s">
         <v>418</v>
       </c>
@@ -46177,6 +46833,9 @@
       </c>
       <c r="S9" t="s">
         <v>247</v>
+      </c>
+      <c r="T9" t="s">
+        <v>434</v>
       </c>
       <c r="U9" t="s">
         <v>419</v>
@@ -46299,7 +46958,7 @@
         <v>549</v>
       </c>
       <c r="O12" t="s">
-        <v>535</v>
+        <v>605</v>
       </c>
       <c r="R12" t="s">
         <v>41</v>
@@ -46335,6 +46994,9 @@
       </c>
       <c r="N13" t="s">
         <v>454</v>
+      </c>
+      <c r="O13" t="s">
+        <v>535</v>
       </c>
       <c r="R13" t="s">
         <v>95</v>
@@ -46413,7 +47075,7 @@
         <v>251</v>
       </c>
       <c r="AA15" t="s">
-        <v>586</v>
+        <v>611</v>
       </c>
       <c r="AD15" t="s">
         <v>195</v>
@@ -46448,7 +47110,7 @@
         <v>252</v>
       </c>
       <c r="AA16" t="s">
-        <v>105</v>
+        <v>586</v>
       </c>
       <c r="AD16" t="s">
         <v>196</v>
@@ -46477,7 +47139,7 @@
         <v>253</v>
       </c>
       <c r="AA17" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="AD17" t="s">
         <v>479</v>
@@ -46503,7 +47165,7 @@
         <v>43</v>
       </c>
       <c r="AA18" t="s">
-        <v>519</v>
+        <v>76</v>
       </c>
       <c r="AF18" t="s">
         <v>493</v>
@@ -46523,7 +47185,7 @@
         <v>471</v>
       </c>
       <c r="AA19" t="s">
-        <v>106</v>
+        <v>519</v>
       </c>
       <c r="AF19" t="s">
         <v>511</v>
@@ -46543,7 +47205,7 @@
         <v>84</v>
       </c>
       <c r="AA20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AF20" t="s">
         <v>512</v>
@@ -46563,7 +47225,7 @@
         <v>85</v>
       </c>
       <c r="AA21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AF21" t="s">
         <v>516</v>
@@ -46583,7 +47245,7 @@
         <v>577</v>
       </c>
       <c r="AA22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AF22" t="s">
         <v>236</v>
@@ -46603,7 +47265,7 @@
         <v>488</v>
       </c>
       <c r="AA23" t="s">
-        <v>500</v>
+        <v>109</v>
       </c>
       <c r="AF23" t="s">
         <v>554</v>
@@ -46623,7 +47285,7 @@
         <v>44</v>
       </c>
       <c r="AA24" t="s">
-        <v>111</v>
+        <v>500</v>
       </c>
       <c r="AF24" t="s">
         <v>555</v>
@@ -46643,7 +47305,7 @@
         <v>400</v>
       </c>
       <c r="AA25" t="s">
-        <v>563</v>
+        <v>111</v>
       </c>
       <c r="AF25" t="s">
         <v>556</v>
@@ -46651,7 +47313,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="F26" t="s">
         <v>463</v>
@@ -46663,7 +47325,7 @@
         <v>541</v>
       </c>
       <c r="AA26" t="s">
-        <v>112</v>
+        <v>563</v>
       </c>
       <c r="AF26" t="s">
         <v>237</v>
@@ -46683,7 +47345,7 @@
         <v>86</v>
       </c>
       <c r="AA27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF27" t="s">
         <v>238</v>
@@ -46703,7 +47365,7 @@
         <v>453</v>
       </c>
       <c r="AA28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29">
@@ -46720,7 +47382,7 @@
         <v>45</v>
       </c>
       <c r="AA29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30">
@@ -46737,7 +47399,7 @@
         <v>46</v>
       </c>
       <c r="AA30" t="s">
-        <v>328</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31">
@@ -46751,7 +47413,7 @@
         <v>217</v>
       </c>
       <c r="AA31" t="s">
-        <v>116</v>
+        <v>328</v>
       </c>
     </row>
     <row r="32">
@@ -46765,7 +47427,7 @@
         <v>276</v>
       </c>
       <c r="AA32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33">
@@ -46776,7 +47438,7 @@
         <v>286</v>
       </c>
       <c r="AA33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34">
@@ -46787,7 +47449,7 @@
         <v>525</v>
       </c>
       <c r="AA34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35">
@@ -46798,7 +47460,7 @@
         <v>261</v>
       </c>
       <c r="AA35" t="s">
-        <v>564</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36">
@@ -46809,7 +47471,7 @@
         <v>331</v>
       </c>
       <c r="AA36" t="s">
-        <v>120</v>
+        <v>564</v>
       </c>
     </row>
     <row r="37">
@@ -46820,7 +47482,7 @@
         <v>308</v>
       </c>
       <c r="AA37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38">
@@ -46831,7 +47493,7 @@
         <v>262</v>
       </c>
       <c r="AA38" t="s">
-        <v>211</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39">
@@ -46842,7 +47504,7 @@
         <v>309</v>
       </c>
       <c r="AA39" t="s">
-        <v>122</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40">
@@ -46850,7 +47512,7 @@
         <v>268</v>
       </c>
       <c r="AA40" t="s">
-        <v>339</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41">
@@ -46858,7 +47520,7 @@
         <v>79</v>
       </c>
       <c r="AA41" t="s">
-        <v>440</v>
+        <v>339</v>
       </c>
     </row>
     <row r="42">
@@ -46866,7 +47528,7 @@
         <v>213</v>
       </c>
       <c r="AA42" t="s">
-        <v>574</v>
+        <v>440</v>
       </c>
     </row>
     <row r="43">
@@ -46874,7 +47536,7 @@
         <v>560</v>
       </c>
       <c r="AA43" t="s">
-        <v>401</v>
+        <v>574</v>
       </c>
     </row>
     <row r="44">
@@ -46882,7 +47544,7 @@
         <v>290</v>
       </c>
       <c r="AA44" t="s">
-        <v>123</v>
+        <v>401</v>
       </c>
     </row>
     <row r="45">
@@ -46890,7 +47552,7 @@
         <v>301</v>
       </c>
       <c r="AA45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46">
@@ -46898,7 +47560,7 @@
         <v>302</v>
       </c>
       <c r="AA46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47">
@@ -46906,7 +47568,7 @@
         <v>344</v>
       </c>
       <c r="AA47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48">
@@ -46914,7 +47576,7 @@
         <v>343</v>
       </c>
       <c r="AA48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49">
@@ -46922,7 +47584,7 @@
         <v>212</v>
       </c>
       <c r="AA49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50">
@@ -46930,7 +47592,7 @@
         <v>321</v>
       </c>
       <c r="AA50" t="s">
-        <v>455</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51">
@@ -46938,7 +47600,7 @@
         <v>340</v>
       </c>
       <c r="AA51" t="s">
-        <v>214</v>
+        <v>612</v>
       </c>
     </row>
     <row r="52">
@@ -46946,7 +47608,7 @@
         <v>369</v>
       </c>
       <c r="AA52" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53">
@@ -46954,7 +47616,7 @@
         <v>303</v>
       </c>
       <c r="AA53" t="s">
-        <v>550</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54">
@@ -46962,7 +47624,7 @@
         <v>357</v>
       </c>
       <c r="AA54" t="s">
-        <v>129</v>
+        <v>550</v>
       </c>
     </row>
     <row r="55">
@@ -46970,7 +47632,7 @@
         <v>332</v>
       </c>
       <c r="AA55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56">
@@ -46978,7 +47640,7 @@
         <v>269</v>
       </c>
       <c r="AA56" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57">
@@ -46986,7 +47648,7 @@
         <v>293</v>
       </c>
       <c r="AA57" t="s">
-        <v>501</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58">
@@ -46994,7 +47656,7 @@
         <v>294</v>
       </c>
       <c r="AA58" t="s">
-        <v>481</v>
+        <v>501</v>
       </c>
     </row>
     <row r="59">
@@ -47002,7 +47664,7 @@
         <v>561</v>
       </c>
       <c r="AA59" t="s">
-        <v>132</v>
+        <v>481</v>
       </c>
     </row>
     <row r="60">
@@ -47010,7 +47672,7 @@
         <v>295</v>
       </c>
       <c r="AA60" t="s">
-        <v>347</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61">
@@ -47018,7 +47680,7 @@
         <v>304</v>
       </c>
       <c r="AA61" t="s">
-        <v>474</v>
+        <v>347</v>
       </c>
     </row>
     <row r="62">
@@ -47026,7 +47688,7 @@
         <v>313</v>
       </c>
       <c r="AA62" t="s">
-        <v>133</v>
+        <v>474</v>
       </c>
     </row>
     <row r="63">
@@ -47034,7 +47696,7 @@
         <v>338</v>
       </c>
       <c r="AA63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64">
@@ -47042,7 +47704,7 @@
         <v>310</v>
       </c>
       <c r="AA64" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65">
@@ -47050,7 +47712,7 @@
         <v>311</v>
       </c>
       <c r="AA65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66">
@@ -47058,7 +47720,7 @@
         <v>370</v>
       </c>
       <c r="AA66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67">
@@ -47066,7 +47728,7 @@
         <v>371</v>
       </c>
       <c r="AA67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68">
@@ -47074,7 +47736,7 @@
         <v>346</v>
       </c>
       <c r="AA68" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69">
@@ -47082,7 +47744,7 @@
         <v>314</v>
       </c>
       <c r="AA69" t="s">
-        <v>451</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70">
@@ -47090,7 +47752,7 @@
         <v>270</v>
       </c>
       <c r="AA70" t="s">
-        <v>491</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71">
@@ -47098,7 +47760,7 @@
         <v>546</v>
       </c>
       <c r="AA71" t="s">
-        <v>215</v>
+        <v>491</v>
       </c>
     </row>
     <row r="72">
@@ -47106,7 +47768,7 @@
         <v>315</v>
       </c>
       <c r="AA72" t="s">
-        <v>397</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73">
@@ -47114,7 +47776,7 @@
         <v>421</v>
       </c>
       <c r="AA73" t="s">
-        <v>456</v>
+        <v>397</v>
       </c>
     </row>
     <row r="74">
@@ -47122,7 +47784,7 @@
         <v>305</v>
       </c>
       <c r="AA74" t="s">
-        <v>140</v>
+        <v>456</v>
       </c>
     </row>
     <row r="75">
@@ -47130,7 +47792,7 @@
         <v>422</v>
       </c>
       <c r="AA75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76">
@@ -47138,7 +47800,7 @@
         <v>263</v>
       </c>
       <c r="AA76" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77">
@@ -47146,7 +47808,7 @@
         <v>526</v>
       </c>
       <c r="AA77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78">
@@ -47154,7 +47816,7 @@
         <v>345</v>
       </c>
       <c r="AA78" t="s">
-        <v>198</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79">
@@ -47162,7 +47824,7 @@
         <v>281</v>
       </c>
       <c r="AA79" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80">
@@ -47170,7 +47832,7 @@
         <v>287</v>
       </c>
       <c r="AA80" t="s">
-        <v>469</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81">
@@ -47178,7 +47840,7 @@
         <v>292</v>
       </c>
       <c r="AA81" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
     </row>
     <row r="82">
@@ -47186,7 +47848,7 @@
         <v>428</v>
       </c>
       <c r="AA82" t="s">
-        <v>144</v>
+        <v>485</v>
       </c>
     </row>
     <row r="83">
@@ -47194,7 +47856,7 @@
         <v>333</v>
       </c>
       <c r="AA83" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84">
@@ -47202,7 +47864,7 @@
         <v>271</v>
       </c>
       <c r="AA84" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85">
@@ -47210,7 +47872,7 @@
         <v>282</v>
       </c>
       <c r="AA85" t="s">
-        <v>513</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86">
@@ -47218,7 +47880,7 @@
         <v>288</v>
       </c>
       <c r="AA86" t="s">
-        <v>147</v>
+        <v>513</v>
       </c>
     </row>
     <row r="87">
@@ -47226,7 +47888,7 @@
         <v>277</v>
       </c>
       <c r="AA87" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="88">
@@ -47234,7 +47896,7 @@
         <v>547</v>
       </c>
       <c r="AA88" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89">
@@ -47242,7 +47904,7 @@
         <v>272</v>
       </c>
       <c r="AA89" t="s">
-        <v>502</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90">
@@ -47250,7 +47912,7 @@
         <v>289</v>
       </c>
       <c r="AA90" t="s">
-        <v>583</v>
+        <v>502</v>
       </c>
     </row>
     <row r="91">
@@ -47258,7 +47920,7 @@
         <v>273</v>
       </c>
       <c r="AA91" t="s">
-        <v>201</v>
+        <v>583</v>
       </c>
     </row>
     <row r="92">
@@ -47266,7 +47928,7 @@
         <v>274</v>
       </c>
       <c r="AA92" t="s">
-        <v>468</v>
+        <v>201</v>
       </c>
     </row>
     <row r="93">
@@ -47274,7 +47936,7 @@
         <v>306</v>
       </c>
       <c r="AA93" t="s">
-        <v>202</v>
+        <v>468</v>
       </c>
     </row>
     <row r="94">
@@ -47282,7 +47944,7 @@
         <v>312</v>
       </c>
       <c r="AA94" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="95">
@@ -47290,7 +47952,7 @@
         <v>296</v>
       </c>
       <c r="AA95" t="s">
-        <v>568</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96">
@@ -47298,7 +47960,7 @@
         <v>341</v>
       </c>
       <c r="AA96" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="97">
@@ -47306,7 +47968,7 @@
         <v>278</v>
       </c>
       <c r="AA97" t="s">
-        <v>216</v>
+        <v>569</v>
       </c>
     </row>
     <row r="98">
@@ -47314,236 +47976,241 @@
         <v>279</v>
       </c>
       <c r="AA98" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="AA99" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="99">
-      <c r="AA99" t="s">
+    <row r="100">
+      <c r="AA100" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="100">
-      <c r="AA100" t="s">
+    <row r="101">
+      <c r="AA101" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="101">
-      <c r="AA101" t="s">
+    <row r="102">
+      <c r="AA102" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="102">
-      <c r="AA102" t="s">
+    <row r="103">
+      <c r="AA103" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="103">
-      <c r="AA103" t="s">
+    <row r="104">
+      <c r="AA104" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="104">
-      <c r="AA104" t="s">
+    <row r="105">
+      <c r="AA105" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="105">
-      <c r="AA105" t="s">
+    <row r="106">
+      <c r="AA106" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="106">
-      <c r="AA106" t="s">
+    <row r="107">
+      <c r="AA107" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="107">
-      <c r="AA107" t="s">
+    <row r="108">
+      <c r="AA108" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="108">
-      <c r="AA108" t="s">
+    <row r="109">
+      <c r="AA109" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="109">
-      <c r="AA109" t="s">
+    <row r="110">
+      <c r="AA110" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="110">
-      <c r="AA110" t="s">
+    <row r="111">
+      <c r="AA111" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="111">
-      <c r="AA111" t="s">
+    <row r="112">
+      <c r="AA112" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="112">
-      <c r="AA112" t="s">
+    <row r="113">
+      <c r="AA113" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="113">
-      <c r="AA113" t="s">
+    <row r="114">
+      <c r="AA114" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="114">
-      <c r="AA114" t="s">
+    <row r="115">
+      <c r="AA115" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="115">
-      <c r="AA115" t="s">
+    <row r="116">
+      <c r="AA116" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="116">
-      <c r="AA116" t="s">
+    <row r="117">
+      <c r="AA117" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="117">
-      <c r="AA117" t="s">
+    <row r="118">
+      <c r="AA118" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="118">
-      <c r="AA118" t="s">
+    <row r="119">
+      <c r="AA119" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="119">
-      <c r="AA119" t="s">
+    <row r="120">
+      <c r="AA120" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="120">
-      <c r="AA120" t="s">
+    <row r="121">
+      <c r="AA121" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="121">
-      <c r="AA121" t="s">
+    <row r="122">
+      <c r="AA122" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="122">
-      <c r="AA122" t="s">
+    <row r="123">
+      <c r="AA123" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="123">
-      <c r="AA123" t="s">
+    <row r="124">
+      <c r="AA124" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="124">
-      <c r="AA124" t="s">
+    <row r="125">
+      <c r="AA125" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="125">
-      <c r="AA125" t="s">
+    <row r="126">
+      <c r="AA126" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="126">
-      <c r="AA126" t="s">
+    <row r="127">
+      <c r="AA127" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="127">
-      <c r="AA127" t="s">
+    <row r="128">
+      <c r="AA128" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="128">
-      <c r="AA128" t="s">
+    <row r="129">
+      <c r="AA129" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="129">
-      <c r="AA129" t="s">
+    <row r="130">
+      <c r="AA130" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="130">
-      <c r="AA130" t="s">
+    <row r="131">
+      <c r="AA131" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="131">
-      <c r="AA131" t="s">
+    <row r="132">
+      <c r="AA132" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="132">
-      <c r="AA132" t="s">
+    <row r="133">
+      <c r="AA133" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="133">
-      <c r="AA133" t="s">
-        <v>457</v>
-      </c>
-    </row>
     <row r="134">
       <c r="AA134" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="AA135" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="135">
-      <c r="AA135" t="s">
+    <row r="136">
+      <c r="AA136" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="136">
-      <c r="AA136" t="s">
+    <row r="137">
+      <c r="AA137" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="137">
-      <c r="AA137" t="s">
+    <row r="138">
+      <c r="AA138" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="138">
-      <c r="AA138" t="s">
+    <row r="139">
+      <c r="AA139" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="139">
-      <c r="AA139" t="s">
+    <row r="140">
+      <c r="AA140" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="140">
-      <c r="AA140" t="s">
+    <row r="141">
+      <c r="AA141" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="141">
-      <c r="AA141" t="s">
+    <row r="142">
+      <c r="AA142" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="142">
-      <c r="AA142" t="s">
+    <row r="143">
+      <c r="AA143" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="143">
-      <c r="AA143" t="s">
+    <row r="144">
+      <c r="AA144" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="144">
-      <c r="AA144" t="s">
+    <row r="145">
+      <c r="AA145" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>